<commit_message>
SCRIPTs - DDL, DML, DQL
</commit_message>
<xml_diff>
--- a/Modelagem/HROADS-FÍSICO.xlsx
+++ b/Modelagem/HROADS-FÍSICO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/480d5ffb018c6fc9/Documentos/SENAI/2DM_Projeto_HROADS/Modelagem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="11_AD4D361C20488DEA4E38A0CD341D69CE5ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02147CC1-6FC2-4691-81CB-9F7569C5E8AD}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="11_AD4D361C20488DEA4E38A0CD341D69CE5ADEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F7E303D-D32E-4374-9C67-E79100023055}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,8 +139,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -323,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -472,6 +480,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,6 +877,9 @@
         <v>44418</v>
       </c>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="59"/>
+    </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
@@ -1013,16 +1025,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K17" s="60"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
@@ -1056,7 +1069,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>2</v>
       </c>
@@ -1073,7 +1086,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>3</v>
       </c>
@@ -1090,7 +1103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>4</v>
       </c>
@@ -1107,7 +1120,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5</v>
       </c>
@@ -1124,7 +1137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>6</v>
       </c>
@@ -1141,7 +1154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>7</v>
       </c>
@@ -1158,7 +1171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>8</v>
       </c>
@@ -1175,7 +1188,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>9</v>
       </c>
@@ -1194,5 +1207,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>